<commit_message>
Creation about the test cases
</commit_message>
<xml_diff>
--- a/Documentation/PTP_Test_Cases_26092023.xlsx
+++ b/Documentation/PTP_Test_Cases_26092023.xlsx
@@ -8,25 +8,323 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutomatizacionPrueba\Documents\Senasoft2023Grupo1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EA8DFC-FA09-4205-A0CA-B6F9BFF4ABC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF7F875-2316-40CB-BA0F-F704ACE5755E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases with Gherkin" sheetId="2" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Step by Step</t>
+  </si>
+  <si>
+    <t>Obtained Result</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Cycle 1</t>
+  </si>
+  <si>
+    <t>Cycle 2</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register with the field empty</t>
+  </si>
+  <si>
+    <t>The registration will be validated correctly with the email.</t>
+  </si>
+  <si>
+    <t>The registration will be validated correctly with Google account.</t>
+  </si>
+  <si>
+    <t>Successful login will be validated via email.</t>
+  </si>
+  <si>
+    <t>Successful login will be validated through the Google account.</t>
+  </si>
+  <si>
+    <t>Incorrect login will be validated with an empty email field.</t>
+  </si>
+  <si>
+    <t>correopruebaSenasoft@gmail.com</t>
+  </si>
+  <si>
+    <t>Your respective Google account</t>
+  </si>
+  <si>
+    <t>User successfully logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jean Pierre </t>
+  </si>
+  <si>
+    <t>Enter the web page
+-Login to the registration module.
+-Enter an unregistered email address.
+-Click on the Continue with email. button.
+-Enter your password.
+-Enter password confirmation.
+-Click on the Create an account button.</t>
+  </si>
+  <si>
+    <t>Feature: Register</t>
+  </si>
+  <si>
+    <t>I as user want to register on the web page</t>
+  </si>
+  <si>
+    <t>Given User is on the web page</t>
+  </si>
+  <si>
+    <t>When User enter the credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then User should see the home page with your account </t>
+  </si>
+  <si>
+    <t>When User enter an empty field</t>
+  </si>
+  <si>
+    <t>Scenario: Succesful Register with Email</t>
+  </si>
+  <si>
+    <t>Scenario: Register with Empty Field</t>
+  </si>
+  <si>
+    <t>Scenario: Register with all Fields Empty</t>
+  </si>
+  <si>
+    <t>When User don't enter a field</t>
+  </si>
+  <si>
+    <t>Scenario: Succesful Register with Google Account</t>
+  </si>
+  <si>
+    <t>And User choose the option of Google</t>
+  </si>
+  <si>
+    <t>Feature: Login</t>
+  </si>
+  <si>
+    <t>I as user want to log in on the web page</t>
+  </si>
+  <si>
+    <t>Scenario: Login with Empty Email</t>
+  </si>
+  <si>
+    <t>When User don't enter your email</t>
+  </si>
+  <si>
+    <t>Then User shouldn't be registered</t>
+  </si>
+  <si>
+    <t>Then User shouldn't be logged in</t>
+  </si>
+  <si>
+    <t>Feature: Accommodation</t>
+  </si>
+  <si>
+    <t>Scenario: Succesful Log in with Email</t>
+  </si>
+  <si>
+    <t>Scenario: Succesful Log in with Google Account</t>
+  </si>
+  <si>
+    <t>I as a user want to look for a hotel for the place I want to go</t>
+  </si>
+  <si>
+    <t>Scenario: Search with an Empty Field</t>
+  </si>
+  <si>
+    <t>Then User should see something information</t>
+  </si>
+  <si>
+    <t>When User enter the information</t>
+  </si>
+  <si>
+    <t>Then User should see the available hotels</t>
+  </si>
+  <si>
+    <t>Succesful Register with Email</t>
+  </si>
+  <si>
+    <t>Succesful Register with Google Account</t>
+  </si>
+  <si>
+    <t>Enter the web page
+-Login to the registration module.
+-Leave the password field empty.
+-Click on the Continue with email. button.</t>
+  </si>
+  <si>
+    <t>Incorrect registration will be validated with an empty password field.</t>
+  </si>
+  <si>
+    <t>Register with all Fields Empty</t>
+  </si>
+  <si>
+    <t>Incorrect registration will be validated with all the empty fields</t>
+  </si>
+  <si>
+    <t>User successfully registered</t>
+  </si>
+  <si>
+    <t>User cannot be registered</t>
+  </si>
+  <si>
+    <t>Succesful Log in with Email</t>
+  </si>
+  <si>
+    <t>Succesful Log in with Google Account</t>
+  </si>
+  <si>
+    <t>Login with Empty Email</t>
+  </si>
+  <si>
+    <t>User not successfully logged in</t>
+  </si>
+  <si>
+    <t>Accommodation</t>
+  </si>
+  <si>
+    <t>Succesful search</t>
+  </si>
+  <si>
+    <t>Search with an Empty Field</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>The accommodation search will be validated with all the fields filled in.</t>
+  </si>
+  <si>
+    <t>Pereira
+12 de Octubre
+4
+0
+2</t>
+  </si>
+  <si>
+    <t>List of hotels and their respective prices</t>
+  </si>
+  <si>
+    <t>12 de Octubre
+4
+0
+2</t>
+  </si>
+  <si>
+    <t>In the lodging search you will not enter the Where we are going field.</t>
+  </si>
+  <si>
+    <t>Notice to fill in the missing field</t>
+  </si>
+  <si>
+    <t>Feature: Languages</t>
+  </si>
+  <si>
+    <t>I as user want to change the language on the web page</t>
+  </si>
+  <si>
+    <t>Scenario: Succesful Search</t>
+  </si>
+  <si>
+    <t>Scenario: Succesful Language Change</t>
+  </si>
+  <si>
+    <t>When User change the language of the web page</t>
+  </si>
+  <si>
+    <t>Then The web page should be in the language of choise</t>
+  </si>
+  <si>
+    <t>Succesful Language Change</t>
+  </si>
+  <si>
+    <t>Changing the language on the page will validate the respective change.</t>
+  </si>
+  <si>
+    <t>The entire page must be in the selected language.</t>
+  </si>
+  <si>
+    <t>The page is in the selected language</t>
+  </si>
+  <si>
+    <t>Enter de web page
+-Login in the accomodation module.
+-Enter the data of where we are going.
+-Enter the date data.
+-Enter the data of the persons.
+-Click on the Search button.</t>
+  </si>
+  <si>
+    <t>Enter de web page
+-Login in the accomodation module.
+-Enter the date data.
+-Enter the data of the persons.
+-Click on the Search button.</t>
+  </si>
+  <si>
+    <t>Enter de web page
+-Click on the flag.
+-Choose the language</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +332,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -51,14 +392,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -336,15 +759,591 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C284502-6405-4FA3-9591-132F73D55EBA}">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="13"/>
+    </row>
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{A38C84D0-7A1E-4D5F-9AD8-26E9D59CA352}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{62017597-C91B-4B94-8A31-B357D3300781}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>